<commit_message>
[kbss-cvut/termit-ui#581] Improve help text in translation imports Excel template.
</commit_message>
<xml_diff>
--- a/src/main/resources/template/termit-translations-import.xlsx
+++ b/src/main/resources/template/termit-translations-import.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Identifikátor</t>
   </si>
@@ -72,12 +72,16 @@
     <t xml:space="preserve">Manual</t>
   </si>
   <si>
-    <t xml:space="preserve">- Pro vícehodnotové položky použijte jako oddělovač středník (;)
-- Pro přidání dalšího jazyka zkopírujte sheet "English" a pojmenujte ho názvem jazyku, který daný sheet reprezentuje</t>
+    <t xml:space="preserve">- Pro vícehodnotové položky použijte jako oddělovač středník (;)</t>
   </si>
   <si>
-    <t xml:space="preserve">- Use a semicolon (;) to separate values in multi-valued attributes
-- To add translations in another language, copy the "English" sheet and label it using the name of the language the sheet will represent</t>
+    <t xml:space="preserve">- Use a semicolon (;) to separate values in multi-valued attributes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Pro přidání dalšího jazyka zkopírujte sheet "English" a pojmenujte ho názvem jazyku, který daný sheet reprezentuje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- To add translations in another language, copy the "English" sheet and label it using the name of the language the sheet will represent</t>
   </si>
   <si>
     <t xml:space="preserve">- Pro jiné jazyky než češtinu a angličtinu použijte anglické názvy sloupců</t>
@@ -86,10 +90,10 @@
     <t xml:space="preserve">- Use English column labels for sheets in languages other than Czech and English</t>
   </si>
   <si>
-    <t xml:space="preserve">- Pojmy mohou být identifikovány pomocí identifikátoru nebo názvu. Pokud chcete pojmy identifikovat pomocí názvu, odstraňte sloupec Identifikátor</t>
+    <t xml:space="preserve">- Pojmy mohou být identifikovány pomocí identifikátoru nebo názvu. Identifikace podle názvu je založena na prvním dostupném sheetu. V něm odstraňte sloupec Identifikátor a ujistěte se, že pojmy s uvedenými názvy v daném jazyce skutečně existují. Záznamy v dalších sheetech budou spárovány s prvním podle řádků. Zjednodušeně řečeno, při identifikaci dle názvu musí první dostupný sheet obsahovat názvy v již existujícím jazyce. Při identifikaci podle identifikátoru můžete sloupec identifikátor použít přímo v sheetu s novými překlady</t>
   </si>
   <si>
-    <t xml:space="preserve">- Term can be identified either by their identifier or their label. If you want to identify terms via their labels, delete the Identifier Column</t>
+    <t xml:space="preserve">- Terms can be identified either by their identifier or their label. Label-based identification uses the first available sheet. In it, delete the Identifier column and ensure that terms with the given labels in the given language indeed exist. Records in other sheets will be paired based on rows numbers. Simply put, when identifying terms by label, the first available sheet must contain labels in an already known language. When using identifier-based identification, the Identifier column can be in the sheet from which translations will be imported</t>
   </si>
   <si>
     <t xml:space="preserve">- Import nijak nezmění existující pojmy a jejich hodnoty, jen přidá překlady</t>
@@ -105,7 +109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -141,6 +145,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -186,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,8 +230,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -246,7 +261,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.27"/>
@@ -8291,7 +8306,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.5"/>
@@ -16331,13 +16346,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="75.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="75.13"/>
@@ -16353,7 +16368,7 @@
       </c>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -16362,8 +16377,8 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -16371,8 +16386,8 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -16380,14 +16395,27 @@
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>